<commit_message>
Agregando atributos a las entidades
</commit_message>
<xml_diff>
--- a/proyecto_entidades_platzi/Paso 2 - relaciones.xlsx
+++ b/proyecto_entidades_platzi/Paso 2 - relaciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CD7880-1D60-41D7-98F8-9A116954E7AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5E20D-D5CD-402C-9E52-3D0FE5181444}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="55">
   <si>
     <t>item</t>
   </si>
@@ -50,6 +50,141 @@
   </si>
   <si>
     <t>1-M</t>
+  </si>
+  <si>
+    <t>ATRIBUTO</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>OBLIGATORIO</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>cuentaPlatzi</t>
+  </si>
+  <si>
+    <t>varchar(60)</t>
+  </si>
+  <si>
+    <t>varchar(80)</t>
+  </si>
+  <si>
+    <t>fechaInicio</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>fechaNacimiento</t>
+  </si>
+  <si>
+    <t>preferencias</t>
+  </si>
+  <si>
+    <t>varchar(300)</t>
+  </si>
+  <si>
+    <t>ITEM</t>
+  </si>
+  <si>
+    <t>nombreItem</t>
+  </si>
+  <si>
+    <t>varchar(40)</t>
+  </si>
+  <si>
+    <t>precioItem</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>stockItem</t>
+  </si>
+  <si>
+    <t>detallesItem</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>METODO DE COMPRA</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>number(40)</t>
+  </si>
+  <si>
+    <t>metodo</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>METODO DE PAGO</t>
+  </si>
+  <si>
+    <t>tipo</t>
+  </si>
+  <si>
+    <t>codPasarela</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>fechaExpiracion</t>
+  </si>
+  <si>
+    <t>PROVEEDOR</t>
+  </si>
+  <si>
+    <t>codCamaraCom</t>
+  </si>
+  <si>
+    <t>fechaUltComp</t>
+  </si>
+  <si>
+    <t>montoUltComp</t>
+  </si>
+  <si>
+    <t>moneda</t>
+  </si>
+  <si>
+    <t>numeroItem</t>
+  </si>
+  <si>
+    <t>comentarios</t>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
   </si>
 </sst>
 </file>
@@ -65,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -78,8 +213,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -102,11 +243,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -117,12 +267,23 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -397,19 +558,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -429,8 +602,20 @@
       <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -452,8 +637,20 @@
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -475,8 +672,20 @@
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -498,8 +707,18 @@
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -521,8 +740,18 @@
       <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -544,8 +773,16 @@
       <c r="H7" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="K7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -567,8 +804,490 @@
       <c r="H8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="K8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="K16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N25" s="1"/>
+    </row>
+    <row r="26" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N26" s="1"/>
+    </row>
+    <row r="27" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K30" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+    </row>
+    <row r="31" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+    </row>
+    <row r="40" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K43" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N43" s="1"/>
+    </row>
+    <row r="44" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N44" s="1"/>
+    </row>
+    <row r="45" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+    </row>
+    <row r="46" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+    </row>
+    <row r="47" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+    </row>
+    <row r="50" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K50" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+    </row>
+    <row r="51" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N52" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K53" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N53" s="1"/>
+    </row>
+    <row r="54" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K54" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+    </row>
+    <row r="55" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K55" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+    </row>
+    <row r="56" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K56" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K50:N50"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregando el proyecto de platzi version 2
</commit_message>
<xml_diff>
--- a/proyecto_entidades_platzi/Paso 2 - relaciones.xlsx
+++ b/proyecto_entidades_platzi/Paso 2 - relaciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762F48E0-0D2F-4C21-9FAF-7B4DD54BC1D2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB89C27-333B-4D40-9C80-DE9811540CD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,9 +97,6 @@
     <t>METODO DE COMPRA</t>
   </si>
   <si>
-    <t>number(40)</t>
-  </si>
-  <si>
     <t>METODO DE PAGO</t>
   </si>
   <si>
@@ -133,91 +130,94 @@
     <t>CARRITO</t>
   </si>
   <si>
-    <t>C_cuentaPlatzi</t>
-  </si>
-  <si>
-    <t>C_nombre</t>
-  </si>
-  <si>
-    <t>C_fechaInicio</t>
-  </si>
-  <si>
-    <t>C_correo</t>
-  </si>
-  <si>
-    <t>C_fechaNacimiento</t>
-  </si>
-  <si>
-    <t>C_preferencias</t>
-  </si>
-  <si>
-    <t>IT_nombreItem</t>
-  </si>
-  <si>
-    <t>IT_precioItem</t>
-  </si>
-  <si>
-    <t>IT_stockItem</t>
-  </si>
-  <si>
-    <t>IT_detallesItem</t>
-  </si>
-  <si>
-    <t>MC_codigo</t>
-  </si>
-  <si>
-    <t>MC_metodo</t>
-  </si>
-  <si>
-    <t>MC_fechaInicio</t>
-  </si>
-  <si>
-    <t>MC_direccion</t>
-  </si>
-  <si>
-    <t>MP_tipo</t>
-  </si>
-  <si>
-    <t>MP_codPasarela</t>
-  </si>
-  <si>
-    <t>MP_status</t>
-  </si>
-  <si>
-    <t>MP_fechaExpiracion</t>
-  </si>
-  <si>
     <t>P_codCamaraCom</t>
   </si>
   <si>
-    <t>P_nombre</t>
-  </si>
-  <si>
-    <t>P_fechaInicio</t>
-  </si>
-  <si>
-    <t>P_fechaUltComp</t>
-  </si>
-  <si>
-    <t>P_montoUltComp</t>
-  </si>
-  <si>
-    <t>P_moneda</t>
-  </si>
-  <si>
     <t>CAR_ID</t>
   </si>
   <si>
-    <t>CAR_numeroItem</t>
-  </si>
-  <si>
-    <t>CAR_direccion</t>
-  </si>
-  <si>
-    <t>CAR_comentarios</t>
-  </si>
-  <si>
     <t>CAR_tag</t>
+  </si>
+  <si>
+    <t>C_accountPlatzi</t>
+  </si>
+  <si>
+    <t>C_name</t>
+  </si>
+  <si>
+    <t>C_startDate</t>
+  </si>
+  <si>
+    <t>C_mail</t>
+  </si>
+  <si>
+    <t>C_birthDate</t>
+  </si>
+  <si>
+    <t>C_preferences</t>
+  </si>
+  <si>
+    <t>IT_name</t>
+  </si>
+  <si>
+    <t>IT_prices</t>
+  </si>
+  <si>
+    <t>IT_stock</t>
+  </si>
+  <si>
+    <t>IT_details</t>
+  </si>
+  <si>
+    <t>MC_code</t>
+  </si>
+  <si>
+    <t>MC_method</t>
+  </si>
+  <si>
+    <t>MC_startDate</t>
+  </si>
+  <si>
+    <t>MC_mail</t>
+  </si>
+  <si>
+    <t>MP_type</t>
+  </si>
+  <si>
+    <t>MP_gatewayCode</t>
+  </si>
+  <si>
+    <t>MP_state</t>
+  </si>
+  <si>
+    <t>MP_expirationDate</t>
+  </si>
+  <si>
+    <t>P_name</t>
+  </si>
+  <si>
+    <t>P_startDate</t>
+  </si>
+  <si>
+    <t>P_lastDatPurcha</t>
+  </si>
+  <si>
+    <t>P_lastPurchAmount</t>
+  </si>
+  <si>
+    <t>P_coin</t>
+  </si>
+  <si>
+    <t>CAR_number</t>
+  </si>
+  <si>
+    <t>CAR_mail</t>
+  </si>
+  <si>
+    <t>CAR_comments</t>
+  </si>
+  <si>
+    <t>number(15)</t>
   </si>
 </sst>
 </file>
@@ -311,11 +311,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,12 +619,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -681,16 +681,16 @@
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -716,16 +716,16 @@
       <c r="H4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N4" s="1" t="s">
+      <c r="M4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -751,16 +751,16 @@
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="K5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N5" s="1"/>
+      <c r="M5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="2"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -784,16 +784,16 @@
       <c r="H6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="K6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6" s="1"/>
+      <c r="M6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N6" s="2"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -818,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L7" s="1" t="s">
         <v>16</v>
@@ -849,7 +849,7 @@
         <v>6</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>18</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K9" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>19</v>
@@ -868,12 +868,12 @@
       <c r="N9" s="1"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="K13" s="1" t="s">
@@ -890,58 +890,58 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="1" t="s">
+      <c r="K14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N14" s="1" t="s">
+      <c r="M14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L15" s="1" t="s">
+      <c r="K15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N15" s="1"/>
+      <c r="M15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N15" s="2"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="K16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="K16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N16" s="1"/>
+      <c r="M16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N16" s="2"/>
     </row>
     <row r="17" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L17" s="1" t="s">
+      <c r="K17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N17" s="1"/>
+      <c r="M17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="2"/>
     </row>
     <row r="18" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K18" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>23</v>
@@ -962,12 +962,12 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K22" s="1" t="s">
@@ -984,60 +984,60 @@
       </c>
     </row>
     <row r="23" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L23" s="1" t="s">
+      <c r="K23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N23" s="1" t="s">
+      <c r="M23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N23" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N24" s="1" t="s">
+      <c r="K24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N24" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L25" s="1" t="s">
+      <c r="K25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N25" s="1"/>
+      <c r="M25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N25" s="2"/>
     </row>
     <row r="26" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L26" s="1" t="s">
+      <c r="K26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N26" s="1"/>
+      <c r="M26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N26" s="2"/>
     </row>
     <row r="27" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K27" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>16</v>
@@ -1058,12 +1058,12 @@
       <c r="N29" s="4"/>
     </row>
     <row r="30" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K30" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
+      <c r="K30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K31" s="1" t="s">
@@ -1080,74 +1080,74 @@
       </c>
     </row>
     <row r="32" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L32" s="1" t="s">
+      <c r="K32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M32" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N32" s="1" t="s">
+      <c r="M32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N32" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K33" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L33" s="1" t="s">
+      <c r="K33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N33" s="1"/>
+      <c r="M33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N33" s="2"/>
     </row>
     <row r="34" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K34" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L34" s="1" t="s">
+      <c r="K34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M34" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N34" s="1"/>
+      <c r="M34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N34" s="2"/>
     </row>
     <row r="35" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="L35" s="1" t="s">
+      <c r="K35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K36" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N36" s="1"/>
-    </row>
-    <row r="39" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K39" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
     </row>
     <row r="40" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K40" s="1" t="s">
@@ -1164,60 +1164,60 @@
       </c>
     </row>
     <row r="41" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K41" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L41" s="1" t="s">
+      <c r="K41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N41" s="1" t="s">
+      <c r="M41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N41" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="42" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N42" s="1" t="s">
+      <c r="K42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N42" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K43" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L43" s="1" t="s">
+      <c r="K43" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N43" s="1"/>
+      <c r="M43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L44" s="1" t="s">
+      <c r="K44" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L44" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N44" s="1"/>
+      <c r="M44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N44" s="2"/>
     </row>
     <row r="45" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K45" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>18</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="46" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K46" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>22</v>
@@ -1237,24 +1237,24 @@
     </row>
     <row r="47" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K47" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
     </row>
     <row r="50" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K50" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
+      <c r="K50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
     </row>
     <row r="51" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K51" s="6" t="s">
+      <c r="K51" s="5" t="s">
         <v>10</v>
       </c>
       <c r="L51" s="1" t="s">
@@ -1268,30 +1268,30 @@
       </c>
     </row>
     <row r="52" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K52" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L52" s="1" t="s">
+      <c r="K52" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N52" s="1" t="s">
+      <c r="M52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N52" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K53" s="1" t="s">
+      <c r="K53" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="L53" s="1" t="s">
+      <c r="L53" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N53" s="1"/>
+      <c r="M53" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N53" s="2"/>
     </row>
     <row r="54" spans="11:14" x14ac:dyDescent="0.25">
       <c r="K54" s="1" t="s">
@@ -1314,11 +1314,11 @@
       <c r="N55" s="1"/>
     </row>
     <row r="56" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K56" s="6" t="s">
-        <v>65</v>
+      <c r="K56" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>

</xml_diff>